<commit_message>
feat: general form date and summary page (#254)
</commit_message>
<xml_diff>
--- a/itech-malawi/forms/app/general_form.xlsx
+++ b/itech-malawi/forms/app/general_form.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="131">
   <si>
     <t>type</t>
   </si>
@@ -114,6 +114,18 @@
     <t>Patient Name</t>
   </si>
   <si>
+    <t>national_id</t>
+  </si>
+  <si>
+    <t>National ID</t>
+  </si>
+  <si>
+    <t>filing_number</t>
+  </si>
+  <si>
+    <t>Filing Number</t>
+  </si>
+  <si>
     <t>phone</t>
   </si>
   <si>
@@ -165,15 +177,99 @@
     <t>../inputs/contact/mpc_no</t>
   </si>
   <si>
-    <t>tracing_outcome</t>
-  </si>
-  <si>
-    <t>Complete this form to capture tracing outcome</t>
+    <t>select_one b2c_outcomes</t>
+  </si>
+  <si>
+    <t>b2c_outcome</t>
+  </si>
+  <si>
+    <t>Back To Care Outcome?</t>
+  </si>
+  <si>
+    <t>explain</t>
+  </si>
+  <si>
+    <t>Please Explain</t>
+  </si>
+  <si>
+    <t>selected(${b2c_outcome}, ‘other’)</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>NO_LABEL</t>
+  </si>
+  <si>
+    <t>(${b2c_outcome} = ‘Dead’ or ${b2c_outcome} = ‘T.O Self’ or ${b2c_outcome} = ‘T.O Official’ or ${b2c_outcome} = ‘Stop ARV self’ or ${b2c_outcome} = ‘Stop ARV Official’)</t>
   </si>
   <si>
     <t>note</t>
   </si>
   <si>
+    <t>selected_outcome</t>
+  </si>
+  <si>
+    <t>Outcome: ${b2c_outcome}</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>date_of_event</t>
+  </si>
+  <si>
+    <t>Date of Event</t>
+  </si>
+  <si>
+    <t>formatted_doe</t>
+  </si>
+  <si>
+    <t>format-date(${date_of_event}, ‘%d-%m-%y’)</t>
+  </si>
+  <si>
+    <t>group_summary</t>
+  </si>
+  <si>
+    <t>Summary page</t>
+  </si>
+  <si>
+    <t>field-list summary</t>
+  </si>
+  <si>
+    <t>_task_label</t>
+  </si>
+  <si>
+    <t>Task Label</t>
+  </si>
+  <si>
+    <t>h1 blue</t>
+  </si>
+  <si>
+    <t>_submit_warning</t>
+  </si>
+  <si>
+    <t>Be sure to submit to complete this action</t>
+  </si>
+  <si>
+    <t>h1</t>
+  </si>
+  <si>
+    <t>_form_description</t>
+  </si>
+  <si>
+    <t>Form description: Complete this form to capture the tracing outcomes.</t>
+  </si>
+  <si>
+    <t>_patient_details</t>
+  </si>
+  <si>
+    <t>Patient Details &lt;I class="fa fa-user”&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>h1 yellow</t>
+  </si>
+  <si>
     <t>contact_name</t>
   </si>
   <si>
@@ -186,34 +282,22 @@
     <t>Patient Phone: ${patient_phone}</t>
   </si>
   <si>
-    <t>contact_mpc_id</t>
-  </si>
-  <si>
-    <t>MPC ID: ${patient_mpc_id}</t>
-  </si>
-  <si>
-    <t>select_one b2c_outcomes</t>
-  </si>
-  <si>
-    <t>b2c_outcome</t>
-  </si>
-  <si>
-    <t>Back To Care Outcome?</t>
-  </si>
-  <si>
-    <t>explain</t>
-  </si>
-  <si>
-    <t>Please Explain</t>
-  </si>
-  <si>
-    <t>selected(${b2c_outcome}, ‘other’)</t>
-  </si>
-  <si>
-    <t>group_summary</t>
-  </si>
-  <si>
-    <t>Summary</t>
+    <t>_national_id</t>
+  </si>
+  <si>
+    <t>National ID: ${national_id}</t>
+  </si>
+  <si>
+    <t>_filing_number</t>
+  </si>
+  <si>
+    <t>Filing Number: ${filing_number}</t>
+  </si>
+  <si>
+    <t>_b2c_outcome</t>
+  </si>
+  <si>
+    <t>Findings</t>
   </si>
   <si>
     <t>outcome</t>
@@ -222,103 +306,61 @@
     <t>Back To Care Outcome: ${b2c_outcome}</t>
   </si>
   <si>
+    <t>_date_of_event</t>
+  </si>
+  <si>
+    <t>Date of Event: ${formatted_doe}</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
     <t>b2c_outcomes</t>
   </si>
   <si>
-    <t>error</t>
-  </si>
-  <si>
     <t xml:space="preserve">Error </t>
   </si>
   <si>
-    <t>file_not_found</t>
-  </si>
-  <si>
     <t>File not found</t>
   </si>
   <si>
-    <t>subsequent_visit</t>
-  </si>
-  <si>
     <t>Subsequent visit</t>
   </si>
   <si>
-    <t>not_traced</t>
-  </si>
-  <si>
     <t>Not traced</t>
   </si>
   <si>
-    <t>tracing_rejected</t>
-  </si>
-  <si>
     <t>Tracing rejected</t>
   </si>
   <si>
-    <t>no_follow_up_attempt</t>
-  </si>
-  <si>
     <t>No follow up attempt</t>
   </si>
   <si>
-    <t>dead</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dead </t>
   </si>
   <si>
-    <t>t_o_self</t>
-  </si>
-  <si>
     <t>T.O Self</t>
   </si>
   <si>
-    <t>t_o_official</t>
-  </si>
-  <si>
     <t>T.O Official</t>
   </si>
   <si>
-    <t>stop_arv_self</t>
-  </si>
-  <si>
     <t>Stop ARV self</t>
   </si>
   <si>
-    <t>stop_arv_official</t>
-  </si>
-  <si>
     <t>Stop ARV Official</t>
   </si>
   <si>
-    <t>refused_to_answer</t>
-  </si>
-  <si>
     <t xml:space="preserve">Refused to Answer </t>
   </si>
   <si>
-    <t>never_started_arv</t>
-  </si>
-  <si>
     <t>Never started ARVs</t>
   </si>
   <si>
-    <t>on_arvs_gap</t>
-  </si>
-  <si>
     <t>On ARVs gaps</t>
   </si>
   <si>
-    <t>on_arvs_no_gap</t>
-  </si>
-  <si>
     <t>On ARVs no gaps</t>
-  </si>
-  <si>
-    <t>other</t>
   </si>
   <si>
     <t>Other</t>
@@ -476,7 +518,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -606,6 +648,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="10"/>
@@ -648,7 +701,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -748,9 +801,6 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="8" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
@@ -766,10 +816,25 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="7" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -793,22 +858,22 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="9" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="9" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1899,7 +1964,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:Z40"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1908,14 +1973,14 @@
     <col min="1" max="1" width="32.6719" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.1719" style="1" customWidth="1"/>
     <col min="3" max="3" width="44.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.3516" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.85156" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.8516" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.8516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6016" style="1" customWidth="1"/>
-    <col min="11" max="11" width="28.4219" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6719" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.8516" style="1" customWidth="1"/>
     <col min="13" max="26" width="11.5" style="1" customWidth="1"/>
     <col min="27" max="16384" width="11.5" style="1" customWidth="1"/>
@@ -2195,7 +2260,7 @@
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" t="s" s="7">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s" s="8">
         <v>33</v>
@@ -2204,7 +2269,9 @@
         <v>34</v>
       </c>
       <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="E8" t="s" s="11">
+        <v>20</v>
+      </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -2229,7 +2296,7 @@
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" t="s" s="7">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s" s="8">
         <v>35</v>
@@ -2238,7 +2305,9 @@
         <v>36</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="E9" t="s" s="11">
+        <v>20</v>
+      </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -2263,10 +2332,14 @@
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
+      <c r="C10" t="s" s="9">
+        <v>38</v>
+      </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -2293,10 +2366,14 @@
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
+        <v>20</v>
+      </c>
+      <c r="B11" t="s" s="8">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s" s="9">
+        <v>40</v>
+      </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -2322,19 +2399,21 @@
       <c r="Z11" s="17"/>
     </row>
     <row r="12" ht="15.35" customHeight="1">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="17"/>
+      <c r="A12" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="16"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
@@ -2350,26 +2429,20 @@
       <c r="Z12" s="17"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
-      <c r="A13" t="s" s="22">
-        <v>38</v>
-      </c>
-      <c r="B13" t="s" s="23">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s" s="24">
-        <v>32</v>
-      </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" t="s" s="24">
-        <v>40</v>
-      </c>
-      <c r="L13" s="26"/>
+      <c r="A13" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
       <c r="M13" s="16"/>
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
@@ -2386,27 +2459,19 @@
       <c r="Z13" s="17"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" t="s" s="22">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s" s="23">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s" s="24">
-        <v>42</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" t="s" s="24">
-        <v>43</v>
-      </c>
-      <c r="L14" s="26"/>
-      <c r="M14" s="16"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="17"/>
       <c r="N14" s="17"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
@@ -2423,13 +2488,13 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="22">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s" s="23">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s" s="24">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
@@ -2439,11 +2504,9 @@
       <c r="I15" s="25"/>
       <c r="J15" s="25"/>
       <c r="K15" t="s" s="24">
-        <v>46</v>
-      </c>
-      <c r="L15" t="s" s="24">
-        <v>20</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="L15" s="26"/>
       <c r="M15" s="16"/>
       <c r="N15" s="17"/>
       <c r="O15" s="17"/>
@@ -2461,13 +2524,13 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" t="s" s="22">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s" s="23">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s" s="24">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
@@ -2477,9 +2540,9 @@
       <c r="I16" s="25"/>
       <c r="J16" s="25"/>
       <c r="K16" t="s" s="24">
-        <v>49</v>
-      </c>
-      <c r="L16" s="24"/>
+        <v>47</v>
+      </c>
+      <c r="L16" s="26"/>
       <c r="M16" s="16"/>
       <c r="N16" s="17"/>
       <c r="O16" s="17"/>
@@ -2496,19 +2559,29 @@
       <c r="Z16" s="17"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="17"/>
+      <c r="A17" t="s" s="22">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s" s="23">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s" s="24">
+        <v>49</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" t="s" s="24">
+        <v>50</v>
+      </c>
+      <c r="L17" t="s" s="24">
+        <v>20</v>
+      </c>
+      <c r="M17" s="16"/>
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
@@ -2523,27 +2596,27 @@
       <c r="Y17" s="17"/>
       <c r="Z17" s="17"/>
     </row>
-    <row r="18" ht="29.25" customHeight="1">
-      <c r="A18" t="s" s="27">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s" s="28">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s" s="29">
+    <row r="18" ht="15.35" customHeight="1">
+      <c r="A18" t="s" s="22">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s" s="23">
         <v>51</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" t="s" s="31">
-        <v>16</v>
-      </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
+      <c r="C18" t="s" s="24">
+        <v>52</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" t="s" s="24">
+        <v>53</v>
+      </c>
+      <c r="L18" s="24"/>
       <c r="M18" s="16"/>
       <c r="N18" s="17"/>
       <c r="O18" s="17"/>
@@ -2559,26 +2632,20 @@
       <c r="Y18" s="17"/>
       <c r="Z18" s="17"/>
     </row>
-    <row r="19" ht="29.25" customHeight="1">
-      <c r="A19" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B19" t="s" s="28">
-        <v>53</v>
-      </c>
-      <c r="C19" t="s" s="29">
-        <v>54</v>
-      </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="16"/>
+    <row r="19" ht="15.35" customHeight="1">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="17"/>
       <c r="P19" s="17"/>
@@ -2595,7 +2662,7 @@
     </row>
     <row r="20" ht="29.25" customHeight="1">
       <c r="A20" t="s" s="27">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s" s="28">
         <v>55</v>
@@ -2605,7 +2672,9 @@
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
+      <c r="F20" t="s" s="31">
+        <v>30</v>
+      </c>
       <c r="G20" s="30"/>
       <c r="H20" s="30"/>
       <c r="I20" s="30"/>
@@ -2629,7 +2698,7 @@
     </row>
     <row r="21" ht="29.25" customHeight="1">
       <c r="A21" t="s" s="27">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s" s="28">
         <v>57</v>
@@ -2637,9 +2706,13 @@
       <c r="C21" t="s" s="29">
         <v>58</v>
       </c>
-      <c r="D21" s="30"/>
+      <c r="D21" t="s" s="31">
+        <v>59</v>
+      </c>
       <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
+      <c r="F21" t="s" s="31">
+        <v>30</v>
+      </c>
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
       <c r="I21" s="30"/>
@@ -2663,7 +2736,7 @@
     </row>
     <row r="22" ht="29.25" customHeight="1">
       <c r="A22" t="s" s="27">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s" s="28">
         <v>60</v>
@@ -2671,11 +2744,13 @@
       <c r="C22" t="s" s="29">
         <v>61</v>
       </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" t="s" s="31">
-        <v>30</v>
-      </c>
+      <c r="D22" t="s" s="31">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s" s="31">
+        <v>16</v>
+      </c>
+      <c r="F22" s="31"/>
       <c r="G22" s="30"/>
       <c r="H22" s="30"/>
       <c r="I22" s="30"/>
@@ -2697,23 +2772,19 @@
       <c r="Y22" s="17"/>
       <c r="Z22" s="17"/>
     </row>
-    <row r="23" ht="29.25" customHeight="1">
+    <row r="23" ht="15.35" customHeight="1">
       <c r="A23" t="s" s="27">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s" s="28">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s" s="29">
-        <v>63</v>
-      </c>
-      <c r="D23" t="s" s="31">
-        <v>64</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D23" s="31"/>
       <c r="E23" s="30"/>
-      <c r="F23" t="s" s="31">
-        <v>30</v>
-      </c>
+      <c r="F23" s="31"/>
       <c r="G23" s="30"/>
       <c r="H23" s="30"/>
       <c r="I23" s="30"/>
@@ -2735,15 +2806,19 @@
       <c r="Y23" s="17"/>
       <c r="Z23" s="17"/>
     </row>
-    <row r="24" ht="29.25" customHeight="1">
+    <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="27">
-        <v>37</v>
-      </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="30"/>
+        <v>66</v>
+      </c>
+      <c r="B24" t="s" s="28">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s" s="29">
+        <v>68</v>
+      </c>
+      <c r="D24" s="31"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="30"/>
       <c r="H24" s="30"/>
       <c r="I24" s="30"/>
@@ -2765,26 +2840,26 @@
       <c r="Y24" s="17"/>
       <c r="Z24" s="17"/>
     </row>
-    <row r="25" ht="27.85" customHeight="1">
+    <row r="25" ht="26.6" customHeight="1">
       <c r="A25" t="s" s="27">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s" s="28">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s" s="29">
-        <v>66</v>
-      </c>
-      <c r="D25" s="30"/>
-      <c r="E25" t="s" s="31">
-        <v>16</v>
-      </c>
-      <c r="F25" s="30"/>
+        <v>61</v>
+      </c>
+      <c r="D25" s="31"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="30"/>
       <c r="H25" s="30"/>
       <c r="I25" s="30"/>
       <c r="J25" s="30"/>
-      <c r="K25" s="32"/>
+      <c r="K25" t="s" s="29">
+        <v>70</v>
+      </c>
       <c r="L25" s="32"/>
       <c r="M25" s="16"/>
       <c r="N25" s="17"/>
@@ -2801,26 +2876,22 @@
       <c r="Y25" s="17"/>
       <c r="Z25" s="17"/>
     </row>
-    <row r="26" ht="15.35" customHeight="1">
+    <row r="26" ht="29.25" customHeight="1">
       <c r="A26" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B26" t="s" s="28">
-        <v>53</v>
-      </c>
-      <c r="C26" t="s" s="34">
-        <v>54</v>
-      </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="17"/>
+        <v>41</v>
+      </c>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="16"/>
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
@@ -2835,26 +2906,28 @@
       <c r="Y26" s="17"/>
       <c r="Z26" s="17"/>
     </row>
-    <row r="27" ht="15.35" customHeight="1">
+    <row r="27" ht="27.85" customHeight="1">
       <c r="A27" t="s" s="27">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s" s="28">
-        <v>55</v>
-      </c>
-      <c r="C27" t="s" s="34">
-        <v>56</v>
-      </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
+        <v>71</v>
+      </c>
+      <c r="C27" t="s" s="29">
+        <v>72</v>
+      </c>
+      <c r="D27" s="30"/>
+      <c r="E27" t="s" s="31">
+        <v>73</v>
+      </c>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="16"/>
       <c r="N27" s="17"/>
       <c r="O27" s="17"/>
       <c r="P27" s="17"/>
@@ -2869,26 +2942,28 @@
       <c r="Y27" s="17"/>
       <c r="Z27" s="17"/>
     </row>
-    <row r="28" ht="15.35" customHeight="1">
+    <row r="28" ht="27.85" customHeight="1">
       <c r="A28" t="s" s="27">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s" s="28">
-        <v>57</v>
-      </c>
-      <c r="C28" t="s" s="34">
-        <v>58</v>
-      </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
+        <v>74</v>
+      </c>
+      <c r="C28" t="s" s="29">
+        <v>75</v>
+      </c>
+      <c r="D28" s="30"/>
+      <c r="E28" t="s" s="31">
+        <v>76</v>
+      </c>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="16"/>
       <c r="N28" s="17"/>
       <c r="O28" s="17"/>
       <c r="P28" s="17"/>
@@ -2903,26 +2978,28 @@
       <c r="Y28" s="17"/>
       <c r="Z28" s="17"/>
     </row>
-    <row r="29" ht="15.35" customHeight="1">
+    <row r="29" ht="27.85" customHeight="1">
       <c r="A29" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B29" t="s" s="39">
-        <v>67</v>
-      </c>
-      <c r="C29" t="s" s="40">
-        <v>68</v>
-      </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
+        <v>63</v>
+      </c>
+      <c r="B29" t="s" s="28">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D29" s="30"/>
+      <c r="E29" t="s" s="31">
+        <v>79</v>
+      </c>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="16"/>
       <c r="N29" s="17"/>
       <c r="O29" s="17"/>
       <c r="P29" s="17"/>
@@ -2937,22 +3014,26 @@
       <c r="Y29" s="17"/>
       <c r="Z29" s="17"/>
     </row>
-    <row r="30" ht="15.35" customHeight="1">
-      <c r="A30" t="s" s="41">
-        <v>37</v>
-      </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
+    <row r="30" ht="27.85" customHeight="1">
+      <c r="A30" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s" s="28">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s" s="29">
+        <v>81</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="16"/>
       <c r="N30" s="17"/>
       <c r="O30" s="17"/>
       <c r="P30" s="17"/>
@@ -2967,20 +3048,28 @@
       <c r="Y30" s="17"/>
       <c r="Z30" s="17"/>
     </row>
-    <row r="31" ht="15.35" customHeight="1">
-      <c r="A31" s="42"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
+    <row r="31" ht="27.85" customHeight="1">
+      <c r="A31" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="B31" t="s" s="28">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s" s="29">
+        <v>83</v>
+      </c>
+      <c r="D31" s="30"/>
+      <c r="E31" t="s" s="31">
+        <v>84</v>
+      </c>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="16"/>
       <c r="N31" s="17"/>
       <c r="O31" s="17"/>
       <c r="P31" s="17"/>
@@ -2994,6 +3083,304 @@
       <c r="X31" s="17"/>
       <c r="Y31" s="17"/>
       <c r="Z31" s="17"/>
+    </row>
+    <row r="32" ht="15.35" customHeight="1">
+      <c r="A32" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="B32" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="C32" t="s" s="33">
+        <v>86</v>
+      </c>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
+    </row>
+    <row r="33" ht="15.35" customHeight="1">
+      <c r="A33" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="C33" t="s" s="33">
+        <v>88</v>
+      </c>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="17"/>
+    </row>
+    <row r="34" ht="15.35" customHeight="1">
+      <c r="A34" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="B34" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s" s="33">
+        <v>90</v>
+      </c>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="17"/>
+      <c r="Z34" s="17"/>
+    </row>
+    <row r="35" ht="15.35" customHeight="1">
+      <c r="A35" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="B35" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s" s="33">
+        <v>92</v>
+      </c>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="17"/>
+      <c r="T35" s="17"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="17"/>
+      <c r="Y35" s="17"/>
+      <c r="Z35" s="17"/>
+    </row>
+    <row r="36" ht="15.35" customHeight="1">
+      <c r="A36" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s" s="28">
+        <v>93</v>
+      </c>
+      <c r="C36" t="s" s="29">
+        <v>94</v>
+      </c>
+      <c r="D36" s="38"/>
+      <c r="E36" t="s" s="39">
+        <v>76</v>
+      </c>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
+      <c r="V36" s="17"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="17"/>
+      <c r="Y36" s="17"/>
+      <c r="Z36" s="17"/>
+    </row>
+    <row r="37" ht="15.35" customHeight="1">
+      <c r="A37" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s" s="41">
+        <v>95</v>
+      </c>
+      <c r="C37" t="s" s="42">
+        <v>96</v>
+      </c>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="17"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="17"/>
+      <c r="Y37" s="17"/>
+      <c r="Z37" s="17"/>
+    </row>
+    <row r="38" ht="15.35" customHeight="1">
+      <c r="A38" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="B38" t="s" s="43">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s" s="44">
+        <v>98</v>
+      </c>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="17"/>
+      <c r="W38" s="17"/>
+      <c r="X38" s="17"/>
+      <c r="Y38" s="17"/>
+      <c r="Z38" s="17"/>
+    </row>
+    <row r="39" ht="15.35" customHeight="1">
+      <c r="A39" t="s" s="45">
+        <v>41</v>
+      </c>
+      <c r="B39" s="36"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="17"/>
+      <c r="W39" s="17"/>
+      <c r="X39" s="17"/>
+      <c r="Y39" s="17"/>
+      <c r="Z39" s="17"/>
+    </row>
+    <row r="40" ht="15.35" customHeight="1">
+      <c r="A40" s="46"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="17"/>
+      <c r="T40" s="17"/>
+      <c r="U40" s="17"/>
+      <c r="V40" s="17"/>
+      <c r="W40" s="17"/>
+      <c r="X40" s="17"/>
+      <c r="Y40" s="17"/>
+      <c r="Z40" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
@@ -3012,243 +3399,243 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="43" customWidth="1"/>
-    <col min="2" max="2" width="20.6719" style="43" customWidth="1"/>
-    <col min="3" max="3" width="36.1719" style="43" customWidth="1"/>
-    <col min="4" max="5" width="11.5" style="43" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="43" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="47" customWidth="1"/>
+    <col min="2" max="2" width="20.6719" style="47" customWidth="1"/>
+    <col min="3" max="3" width="36.1719" style="47" customWidth="1"/>
+    <col min="4" max="5" width="11.5" style="47" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" t="s" s="44">
-        <v>69</v>
-      </c>
-      <c r="B1" t="s" s="44">
+      <c r="A1" t="s" s="48">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s" s="48">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="44">
+      <c r="C1" t="s" s="48">
         <v>2</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
     </row>
     <row r="2" ht="15.35" customHeight="1">
-      <c r="A2" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B2" t="s" s="46">
-        <v>71</v>
-      </c>
-      <c r="C2" t="s" s="46">
-        <v>72</v>
+      <c r="A2" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s" s="50">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s" s="50">
+        <v>101</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
     </row>
     <row r="3" ht="15.35" customHeight="1">
-      <c r="A3" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B3" t="s" s="46">
-        <v>73</v>
-      </c>
-      <c r="C3" t="s" s="46">
-        <v>74</v>
+      <c r="A3" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s" s="50">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s" s="50">
+        <v>102</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
     </row>
     <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B4" t="s" s="46">
-        <v>75</v>
-      </c>
-      <c r="C4" t="s" s="46">
-        <v>76</v>
+      <c r="A4" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s" s="50">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s" s="50">
+        <v>103</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B5" t="s" s="46">
-        <v>77</v>
-      </c>
-      <c r="C5" t="s" s="46">
-        <v>78</v>
+      <c r="A5" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s" s="50">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s" s="50">
+        <v>104</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
     <row r="6" ht="15.35" customHeight="1">
-      <c r="A6" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B6" t="s" s="46">
-        <v>79</v>
-      </c>
-      <c r="C6" t="s" s="46">
-        <v>80</v>
+      <c r="A6" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s" s="50">
+        <v>105</v>
+      </c>
+      <c r="C6" t="s" s="50">
+        <v>105</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
     </row>
     <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B7" t="s" s="46">
-        <v>81</v>
-      </c>
-      <c r="C7" t="s" s="46">
-        <v>82</v>
+      <c r="A7" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s" s="50">
+        <v>106</v>
+      </c>
+      <c r="C7" t="s" s="50">
+        <v>106</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
-      <c r="A8" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B8" t="s" s="46">
-        <v>83</v>
-      </c>
-      <c r="C8" t="s" s="46">
-        <v>84</v>
+      <c r="A8" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s" s="50">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s" s="50">
+        <v>107</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B9" t="s" s="46">
-        <v>85</v>
-      </c>
-      <c r="C9" t="s" s="46">
-        <v>86</v>
+      <c r="A9" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s" s="50">
+        <v>108</v>
+      </c>
+      <c r="C9" t="s" s="50">
+        <v>108</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B10" t="s" s="46">
-        <v>87</v>
-      </c>
-      <c r="C10" t="s" s="46">
-        <v>88</v>
+      <c r="A10" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s" s="50">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s" s="50">
+        <v>109</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
     </row>
     <row r="11" ht="15.35" customHeight="1">
-      <c r="A11" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B11" t="s" s="46">
-        <v>89</v>
-      </c>
-      <c r="C11" t="s" s="46">
-        <v>90</v>
+      <c r="A11" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B11" t="s" s="50">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s" s="50">
+        <v>110</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
     </row>
     <row r="12" ht="15.35" customHeight="1">
-      <c r="A12" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B12" t="s" s="46">
-        <v>91</v>
-      </c>
-      <c r="C12" t="s" s="46">
-        <v>92</v>
+      <c r="A12" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B12" t="s" s="50">
+        <v>111</v>
+      </c>
+      <c r="C12" t="s" s="50">
+        <v>111</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
-      <c r="A13" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B13" t="s" s="46">
-        <v>93</v>
-      </c>
-      <c r="C13" t="s" s="46">
-        <v>94</v>
+      <c r="A13" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B13" t="s" s="50">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s" s="50">
+        <v>112</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B14" t="s" s="46">
-        <v>95</v>
-      </c>
-      <c r="C14" t="s" s="46">
-        <v>96</v>
+      <c r="A14" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s" s="50">
+        <v>113</v>
+      </c>
+      <c r="C14" t="s" s="50">
+        <v>113</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
-      <c r="A15" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B15" t="s" s="46">
-        <v>97</v>
-      </c>
-      <c r="C15" t="s" s="46">
-        <v>98</v>
+      <c r="A15" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B15" t="s" s="50">
+        <v>114</v>
+      </c>
+      <c r="C15" t="s" s="50">
+        <v>114</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B16" t="s" s="46">
-        <v>99</v>
-      </c>
-      <c r="C16" t="s" s="46">
+      <c r="A16" t="s" s="49">
         <v>100</v>
+      </c>
+      <c r="B16" t="s" s="50">
+        <v>115</v>
+      </c>
+      <c r="C16" t="s" s="50">
+        <v>115</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
-      <c r="A17" t="s" s="45">
-        <v>70</v>
-      </c>
-      <c r="B17" t="s" s="46">
-        <v>101</v>
-      </c>
-      <c r="C17" t="s" s="46">
-        <v>102</v>
+      <c r="A17" t="s" s="49">
+        <v>100</v>
+      </c>
+      <c r="B17" t="s" s="50">
+        <v>116</v>
+      </c>
+      <c r="C17" t="s" s="50">
+        <v>116</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
-      <c r="A18" s="45"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" s="45"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -3285,104 +3672,104 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="32" style="47" customWidth="1"/>
-    <col min="2" max="2" width="43.8516" style="47" customWidth="1"/>
-    <col min="3" max="3" width="32.8516" style="47" customWidth="1"/>
-    <col min="4" max="4" width="20.8516" style="47" customWidth="1"/>
-    <col min="5" max="15" width="11.5" style="47" customWidth="1"/>
-    <col min="16" max="26" width="8.85156" style="47" customWidth="1"/>
-    <col min="27" max="16384" width="11.5" style="47" customWidth="1"/>
+    <col min="1" max="1" width="32" style="51" customWidth="1"/>
+    <col min="2" max="2" width="43.8516" style="51" customWidth="1"/>
+    <col min="3" max="3" width="32.8516" style="51" customWidth="1"/>
+    <col min="4" max="4" width="20.8516" style="51" customWidth="1"/>
+    <col min="5" max="15" width="11.5" style="51" customWidth="1"/>
+    <col min="16" max="26" width="8.85156" style="51" customWidth="1"/>
+    <col min="27" max="16384" width="11.5" style="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
-      <c r="A1" t="s" s="48">
-        <v>103</v>
-      </c>
-      <c r="B1" t="s" s="48">
-        <v>104</v>
-      </c>
-      <c r="C1" t="s" s="48">
-        <v>105</v>
-      </c>
-      <c r="D1" t="s" s="48">
-        <v>106</v>
-      </c>
-      <c r="E1" t="s" s="48">
-        <v>107</v>
-      </c>
-      <c r="F1" t="s" s="48">
-        <v>108</v>
-      </c>
-      <c r="G1" t="s" s="48">
+      <c r="A1" t="s" s="52">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s" s="52">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s" s="52">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s" s="52">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s" s="52">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s" s="52">
+        <v>122</v>
+      </c>
+      <c r="G1" t="s" s="52">
         <v>1</v>
       </c>
-      <c r="H1" t="s" s="48">
-        <v>109</v>
-      </c>
-      <c r="I1" t="s" s="48">
-        <v>110</v>
-      </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49"/>
+      <c r="H1" t="s" s="52">
+        <v>123</v>
+      </c>
+      <c r="I1" t="s" s="52">
+        <v>124</v>
+      </c>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" t="s" s="50">
-        <v>111</v>
-      </c>
-      <c r="B2" t="s" s="51">
-        <v>112</v>
-      </c>
-      <c r="C2" s="52">
+      <c r="A2" t="s" s="54">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s" s="55">
+        <v>126</v>
+      </c>
+      <c r="C2" s="56">
         <v>43008</v>
       </c>
-      <c r="D2" t="s" s="51">
-        <v>113</v>
-      </c>
-      <c r="E2" t="s" s="51">
-        <v>114</v>
-      </c>
-      <c r="F2" s="53"/>
-      <c r="G2" t="s" s="51">
-        <v>115</v>
-      </c>
-      <c r="H2" t="s" s="51">
-        <v>115</v>
-      </c>
-      <c r="I2" t="s" s="51">
-        <v>116</v>
-      </c>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
+      <c r="D2" t="s" s="55">
+        <v>127</v>
+      </c>
+      <c r="E2" t="s" s="55">
+        <v>128</v>
+      </c>
+      <c r="F2" s="57"/>
+      <c r="G2" t="s" s="55">
+        <v>129</v>
+      </c>
+      <c r="H2" t="s" s="55">
+        <v>129</v>
+      </c>
+      <c r="I2" t="s" s="55">
+        <v>130</v>
+      </c>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+      <c r="Z2" s="57"/>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" s="17"/>

</xml_diff>